<commit_message>
Avance y renacer del proyecto :P
</commit_message>
<xml_diff>
--- a/ClinicalSheet2_0/data/Documentos/Libro1.xlsx
+++ b/ClinicalSheet2_0/data/Documentos/Libro1.xlsx
@@ -9,22 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>David</t>
   </si>
@@ -32,10 +27,16 @@
     <t>Reyes Alvarado</t>
   </si>
   <si>
+    <t>1013643921</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
     <t>Octubre</t>
   </si>
   <si>
-    <t>06</t>
+    <t>1993</t>
   </si>
   <si>
     <t>Soyelmejor123</t>
@@ -48,7 +49,7 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,9 +75,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,45 +360,35 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.42578125" style="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
-        <v>1013643921</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1993</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D1" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>